<commit_message>
txt to csv_VD dataset
</commit_message>
<xml_diff>
--- a/Exploration_for_VD_dataset/meas_time_edf_hypno.xlsx
+++ b/Exploration_for_VD_dataset/meas_time_edf_hypno.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\code_mine\Exploration_for_VD_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0D675596-BE2A-4131-A79A-6838F1528AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12659E97-B0D2-4A08-B2D2-E047596F7E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meas_time_edf_hypno" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>hypno_start</t>
   </si>
@@ -193,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -780,11 +793,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,14 +848,7 @@
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1184,11 +1193,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1196,7 +1205,7 @@
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1218,8 +1227,14 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1245,8 +1260,20 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="Q2">
+        <v>0.24459490740740741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1272,8 +1299,20 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0.27534722222222224</v>
+      </c>
+      <c r="Q3">
+        <v>0.27598379629629627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1299,8 +1338,20 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="Q4">
+        <v>0.2825347222222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1326,8 +1377,20 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="Q5">
+        <v>0.25601851851851853</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1353,8 +1416,20 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>0.26284722222222223</v>
+      </c>
+      <c r="Q6">
+        <v>0.26346064814814812</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1380,8 +1455,20 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>0.2590277777777778</v>
+      </c>
+      <c r="Q7">
+        <v>0.2592592592592593</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1407,8 +1494,20 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="Q8">
+        <v>0.25581018518518517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1434,8 +1533,20 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="Q9">
+        <v>0.24042824074074076</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1461,8 +1572,21 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>0.28958333333333336</v>
+      </c>
+      <c r="Q10">
+        <f>1.29446759259259-1</f>
+        <v>0.29446759259258992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1488,8 +1612,20 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>0.25833333333333336</v>
+      </c>
+      <c r="Q11">
+        <v>1.2584143518518518</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1515,8 +1651,20 @@
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="L12">
+        <v>11</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0.28506944444444443</v>
+      </c>
+      <c r="Q12">
+        <v>1.2851504629629629</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1542,8 +1690,14 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P13">
+        <v>0.27604166666666669</v>
+      </c>
+      <c r="Q13">
+        <v>1.2761689814814816</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1569,8 +1723,14 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P14">
+        <v>0.27812500000000001</v>
+      </c>
+      <c r="Q14">
+        <v>1.2784837962962963</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1596,8 +1756,14 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P15">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="Q15">
+        <v>1.2669097222222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1623,8 +1789,14 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P16">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="Q16">
+        <v>1.2732291666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1650,8 +1822,14 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P17">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="Q17">
+        <v>1.2801736111111111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1677,8 +1855,14 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P18">
+        <v>0.27118055555555554</v>
+      </c>
+      <c r="Q18">
+        <v>1.2712037037037036</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1704,8 +1888,14 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="Q19">
+        <v>1.2711111111111113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1731,8 +1921,14 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P20">
+        <v>0.28125</v>
+      </c>
+      <c r="Q20">
+        <v>1.281412037037037</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1758,8 +1954,14 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P21">
+        <v>0.25069444444444444</v>
+      </c>
+      <c r="Q21">
+        <v>1.2510416666666666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1785,8 +1987,14 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P22">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="Q22">
+        <v>1.2738194444444444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1812,8 +2020,14 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P23">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="Q23">
+        <v>1.2710185185185185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1839,8 +2053,18 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K24" t="b">
+        <f>C25&gt;F25</f>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0.27256944444444448</v>
+      </c>
+      <c r="Q24">
+        <v>1.2729629629629629</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1866,8 +2090,14 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P25">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="Q25">
+        <v>1.2735879629629629</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1893,8 +2123,14 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P26">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="Q26">
+        <v>1.2272569444444443</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1920,8 +2156,14 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P27">
+        <v>0.27881944444444445</v>
+      </c>
+      <c r="Q27">
+        <v>1.2793287037037038</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1947,8 +2189,14 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P28">
+        <v>0.27638888888888885</v>
+      </c>
+      <c r="Q28">
+        <v>1.276712962962963</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1974,8 +2222,14 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P29">
+        <v>0.29583333333333334</v>
+      </c>
+      <c r="Q29">
+        <v>1.2972337962962963</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2001,8 +2255,14 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P30">
+        <v>0.25590277777777776</v>
+      </c>
+      <c r="Q30">
+        <v>1.2571064814814814</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2028,8 +2288,14 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P31">
+        <v>0.27118055555555554</v>
+      </c>
+      <c r="Q31">
+        <v>1.2712268518518519</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2055,8 +2321,14 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P32">
+        <v>0.3107638888888889</v>
+      </c>
+      <c r="Q32">
+        <v>1.3112731481481481</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2082,8 +2354,14 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P33">
+        <v>0.29131944444444446</v>
+      </c>
+      <c r="Q33">
+        <v>1.2925694444444444</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2109,8 +2387,14 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P34">
+        <v>0.328125</v>
+      </c>
+      <c r="Q34">
+        <v>1.3287847222222222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2136,8 +2420,14 @@
       <c r="H35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P35">
+        <v>0.27604166666666669</v>
+      </c>
+      <c r="Q35">
+        <v>1.2771874999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2163,8 +2453,14 @@
       <c r="H36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P36">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Q36">
+        <v>1.2529629629629631</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2190,8 +2486,14 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P37">
+        <v>0.25347222222222221</v>
+      </c>
+      <c r="Q37">
+        <v>1.2538194444444444</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2217,8 +2519,14 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P38">
+        <v>0.25034722222222222</v>
+      </c>
+      <c r="Q38">
+        <v>1.2507407407407407</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2244,8 +2552,14 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P39">
+        <v>0.22951388888888888</v>
+      </c>
+      <c r="Q39">
+        <v>1.2297800925925926</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2271,8 +2585,14 @@
       <c r="H40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P40">
+        <v>0.27187500000000003</v>
+      </c>
+      <c r="Q40">
+        <v>1.2727777777777778</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2298,8 +2618,14 @@
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P41">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="Q41">
+        <v>1.2642592592592594</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2325,8 +2651,14 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P42">
+        <v>0.26909722222222221</v>
+      </c>
+      <c r="Q42">
+        <v>1.2704166666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2352,8 +2684,14 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P43">
+        <v>0.28576388888888887</v>
+      </c>
+      <c r="Q43">
+        <v>1.2867708333333334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2379,8 +2717,14 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P44">
+        <v>0.29930555555555555</v>
+      </c>
+      <c r="Q44">
+        <v>1.2996875000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2406,8 +2750,14 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P45">
+        <v>0.25347222222222221</v>
+      </c>
+      <c r="Q45">
+        <v>1.2537499999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2433,8 +2783,14 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P46">
+        <v>0.2454861111111111</v>
+      </c>
+      <c r="Q46">
+        <v>1.2466666666666666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2460,8 +2816,14 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P47">
+        <v>0.27013888888888887</v>
+      </c>
+      <c r="Q47">
+        <v>1.272013888888889</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2487,8 +2849,14 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P48">
+        <v>0.25</v>
+      </c>
+      <c r="Q48">
+        <v>1.2504629629629629</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2514,8 +2882,14 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="P49">
+        <v>0.265625</v>
+      </c>
+      <c r="Q49">
+        <v>1.266377314814815</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2541,17 +2915,1447 @@
       <c r="H50">
         <v>0</v>
       </c>
+      <c r="P50">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Q50">
+        <v>1.2534490740740742</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G92" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G93" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G94" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G95" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G97" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G98" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G99" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G100" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B50">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>$B$2&lt;$D$2</formula>
+  <conditionalFormatting sqref="L2:L12">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$L2&gt;$N2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C50">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$P2&gt;$Q2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B45D443-12C7-4221-AFC3-FFC63056F38F}">
+  <dimension ref="B2:I51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.1527777777777781E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.24444444444444446</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.2349537037037039E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.23224537037037038</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3+F3</f>
+        <v>0.24459490740740741</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.7013888888888887E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.27534722222222224</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.1469907407407408E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.26451388888888888</v>
+      </c>
+      <c r="G4" s="2">
+        <f>E4+F4</f>
+        <v>0.27598379629629627</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7.3958333333333341E-3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.27513888888888888</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G10" si="0">E5+F5</f>
+        <v>0.2825347222222222</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.7013888888888887E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.300925925925926E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.24300925925925929</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25601851851851853</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.26284722222222223</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8.5069444444444437E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.25495370370370368</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26346064814814812</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.7013888888888887E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.2590277777777778</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.3402777777777777E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.24585648148148151</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2592592592592593</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.238425925925926E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.23342592592592593</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25581018518518517</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.326388888888889E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.2858796296296294E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.21756944444444445</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24042824074074076</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.5972222222222222E-3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.28958333333333336</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.750462962962963</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.54400462962962959</v>
+      </c>
+      <c r="G11" s="2">
+        <f>E11+F11-1</f>
+        <v>0.29446759259259259</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.25833333333333336</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.74957175925925934</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.50884259259259257</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" ref="G12:G51" si="1">E12+F12-1</f>
+        <v>0.2584143518518518</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.8402777777777778E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.28506944444444443</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.75866898148148154</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.52648148148148144</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28515046296296287</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.27604166666666669</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.75468750000000007</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.52148148148148155</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27616898148148161</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.27812500000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.74690972222222218</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.53157407407407409</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27848379629629627</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.78170138888888896</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.4852083333333333</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26690972222222231</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.75392361111111106</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.51930555555555558</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27322916666666663</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5.1736111111111115E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.79311342592592593</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.48706018518518518</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28017361111111105</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.27118055555555554</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.77722222222222215</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.49398148148148152</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27120370370370361</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4.5138888888888893E-3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.7475925925925927</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.52351851851851849</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2711111111111113</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.28125</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.76974537037037039</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.5116666666666666</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28141203703703699</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.25069444444444444</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.74840277777777775</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.50263888888888886</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25104166666666661</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.76768518518518514</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.50613425925925926</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27381944444444439</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.99895833333333339</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.76585648148148155</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.50516203703703699</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27101851851851855</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="2">
+        <v>9.3749999999999997E-3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.27256944444444448</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.77909722222222222</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.49386574074074074</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27296296296296285</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.0069444444444445E-2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.76168981481481479</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.51189814814814816</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27358796296296295</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.9791666666666666E-2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.7790393518518518</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.44821759259259258</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22725694444444433</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2">
+        <v>7.2916666666666659E-3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.27881944444444445</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.75016203703703699</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27932870370370377</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.27638888888888885</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.74624999999999997</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.53046296296296302</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27671296296296299</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2.9513888888888892E-2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.29583333333333334</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.76586805555555559</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.53136574074074072</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.29723379629629632</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.25590277777777776</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.74946759259259255</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.50763888888888886</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25710648148148141</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.27118055555555554</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.7732175925925926</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.49800925925925926</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27122685185185191</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.3107638888888889</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.75766203703703694</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.55361111111111116</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>0.3112731481481481</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.29131944444444446</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.76504629629629628</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.52752314814814816</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.29256944444444444</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.328125</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.77519675925925924</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.55358796296296298</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>0.32878472222222221</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.27604166666666669</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.78547453703703696</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.49171296296296302</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27718749999999992</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="2">
+        <v>7.2916666666666659E-3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.76050925925925927</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.49245370370370373</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25296296296296306</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2.2569444444444444E-2</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.25347222222222221</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.76189814814814805</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.49192129629629627</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25381944444444438</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="2">
+        <v>3.784722222222222E-2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.25034722222222222</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.79437500000000005</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.45636574074074071</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25074074074074071</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.22951388888888888</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.74954861111111104</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.48023148148148148</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22978009259259258</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="2">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.27187500000000003</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.82370370370370372</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.44907407407407413</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27277777777777779</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.76337962962962969</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.50087962962962962</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26425925925925942</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.26909722222222221</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.79537037037037039</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.4750462962962963</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27041666666666675</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.28576388888888887</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.78431712962962974</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.50245370370370368</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28677083333333342</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.29930555555555555</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.79093750000000007</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.50875000000000004</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="1"/>
+        <v>0.29968750000000011</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3.1249999999999997E-3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.25347222222222221</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.74685185185185177</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.50689814814814815</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25374999999999992</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.2454861111111111</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.74567129629629625</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.50099537037037034</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24666666666666659</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="2">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.27013888888888887</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.81481481481481488</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.45719907407407406</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="1"/>
+        <v>0.272013888888889</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.74914351851851846</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.50131944444444443</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25046296296296289</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="2">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.265625</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.79040509259259262</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.47597222222222224</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26637731481481497</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.75870370370370377</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.49474537037037036</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25344907407407424</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="D3:D51">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$C$2&gt;$F$2</formula>
+      <formula>$D3&gt;$G3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$P3&gt;$Q3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$C3&lt;$E3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>